<commit_message>
new rooms page and functionality
</commit_message>
<xml_diff>
--- a/GUI_App/StudentRegistration.xlsx
+++ b/GUI_App/StudentRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MacEwan\CMPT 395\Project\2023-01_Team3_VLAD\GUI_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B29FC3-7212-4EC8-A9C2-EAACE6C2AC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654D5DFE-4E4A-45E5-8494-2854CE27CAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95899252-5A3F-4CD2-B1DD-5D2B171E3977}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95899252-5A3F-4CD2-B1DD-5D2B171E3977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Professional Communication (PCOM)</t>
   </si>
@@ -61,13 +61,46 @@
   </si>
   <si>
     <t>3rd Term Students</t>
+  </si>
+  <si>
+    <t>Classroom #</t>
+  </si>
+  <si>
+    <t>Normal Capacity</t>
+  </si>
+  <si>
+    <t>11-533</t>
+  </si>
+  <si>
+    <t>11-534</t>
+  </si>
+  <si>
+    <t>11-560</t>
+  </si>
+  <si>
+    <t>11-562</t>
+  </si>
+  <si>
+    <t>11-564</t>
+  </si>
+  <si>
+    <t>11-458</t>
+  </si>
+  <si>
+    <t>11-320</t>
+  </si>
+  <si>
+    <t>11-532 Computer Lab</t>
+  </si>
+  <si>
+    <t>11-430</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,16 +114,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -98,12 +145,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3A8F9F-3097-4177-9B21-9943BD27B337}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,25 +570,25 @@
     <col min="1" max="1" width="37.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -456,12 +597,12 @@
       <c r="C2">
         <v>133</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -470,60 +611,54 @@
       <c r="C3">
         <v>39</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <f>38+37+27</f>
         <v>102</v>
       </c>
       <c r="C4">
-        <f>24+24+25</f>
         <v>73</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <f>27+24+23</f>
         <v>74</v>
       </c>
       <c r="C5">
-        <f>21+20+22</f>
         <v>63</v>
       </c>
-      <c r="D5">
-        <f>16+15</f>
+      <c r="D5" s="5">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <f>21+20</f>
         <v>41</v>
       </c>
       <c r="C6">
         <v>18</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -532,12 +667,12 @@
       <c r="C7">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -546,22 +681,103 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="7">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="8">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>